<commit_message>
done utilization analysis for design before optimizing buffer issue
</commit_message>
<xml_diff>
--- a/doc/report from Vivado/Util Compare Ver2.xlsx
+++ b/doc/report from Vivado/Util Compare Ver2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>N</t>
   </si>
@@ -40,7 +40,13 @@
     <t>LUTs growth V2</t>
   </si>
   <si>
+    <t>LUTs growth V3</t>
+  </si>
+  <si>
     <t>FFs growth V2</t>
+  </si>
+  <si>
+    <t>FFs growth V3</t>
   </si>
   <si>
     <t>LUTs Percentage V1</t>
@@ -66,10 +72,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -81,7 +87,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -94,6 +100,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="等线"/>
@@ -101,8 +115,54 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -124,6 +184,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -133,7 +201,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -141,61 +209,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -209,16 +223,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -233,7 +239,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -245,13 +275,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -263,103 +347,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -377,43 +371,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -446,7 +452,16 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -458,6 +473,15 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -477,20 +501,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -509,31 +530,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -542,133 +548,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -795,7 +801,7 @@
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="0"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$B$1</c:f>
@@ -891,15 +897,15 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:idx val="0"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Sheet1!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Overall LUTs V2</c:v>
+                  <c:v>Overall LUTs V3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -907,7 +913,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -954,7 +960,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$9</c:f>
+              <c:f>Sheet1!$D$2:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -962,25 +968,25 @@
                   <c:v>830</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>874</c:v>
+                  <c:v>867</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>880</c:v>
+                  <c:v>872</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1035</c:v>
+                  <c:v>1003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1228</c:v>
+                  <c:v>1216</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1715</c:v>
+                  <c:v>1669</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2431</c:v>
+                  <c:v>2206</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4129</c:v>
+                  <c:v>3608</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1003,21 +1009,21 @@
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
               <c15:ser>
-                <c:idx val="0"/>
-                <c:order val="0"/>
+                <c:idx val="2"/>
+                <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$A$1</c15:sqref>
+                          <c15:sqref>Sheet1!$C$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>N</c:v>
+                        <c:v>Overall LUTs V2</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -1025,7 +1031,7 @@
                 <c:spPr>
                   <a:ln w="28575" cap="rnd">
                     <a:solidFill>
-                      <a:schemeClr val="accent1"/>
+                      <a:schemeClr val="accent3"/>
                     </a:solidFill>
                     <a:round/>
                   </a:ln>
@@ -1084,7 +1090,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$A$2:$A$9</c15:sqref>
+                          <c15:sqref>Sheet1!$C$2:$C$9</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1092,28 +1098,28 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="8"/>
                       <c:pt idx="0">
-                        <c:v>1</c:v>
+                        <c:v>830</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>2</c:v>
+                        <c:v>874</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>3</c:v>
+                        <c:v>880</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>6</c:v>
+                        <c:v>1035</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>11</c:v>
+                        <c:v>1228</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>22</c:v>
+                        <c:v>1715</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>33</c:v>
+                        <c:v>2431</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>66</c:v>
+                        <c:v>4129</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1124,7 +1130,7 @@
             <c15:filteredLineSeries>
               <c15:ser>
                 <c:idx val="3"/>
-                <c:order val="3"/>
+                <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
                     <c:extLst>
@@ -1244,7 +1250,7 @@
             <c15:filteredLineSeries>
               <c15:ser>
                 <c:idx val="4"/>
-                <c:order val="4"/>
+                <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
                     <c:extLst>
@@ -1698,15 +1704,15 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
+          <c:idx val="5"/>
+          <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$1</c:f>
+              <c:f>Sheet1!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Overall FFs V2</c:v>
+                  <c:v>Overall FFs V3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1714,7 +1720,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent5"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1761,7 +1767,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>{1002,1031,1046,1133,1278,1597,1918,2875}</c:f>
+              <c:f>Sheet1!$G$2:$G$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1769,25 +1775,25 @@
                   <c:v>1002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1031</c:v>
+                  <c:v>1023</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1046</c:v>
+                  <c:v>1030</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1133</c:v>
+                  <c:v>1093</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1278</c:v>
+                  <c:v>1198</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1597</c:v>
+                  <c:v>1429</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1918</c:v>
+                  <c:v>1662</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2875</c:v>
+                  <c:v>2355</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2168,9 +2174,1828 @@
                 <c:smooth val="0"/>
               </c15:ser>
             </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="4"/>
+                <c:order val="4"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$F$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Overall FFs V2</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent5"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:dLbls>
+                  <c:delete val="1"/>
+                </c:dLbls>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref/>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$2:$A$9</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>33</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>66</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>{1002,1031,1046,1133,1278,1597,1918,2875}</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>1002</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1031</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1046</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1133</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1278</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1597</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>1918</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>2875</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+              </c15:ser>
+            </c15:filteredLineSeries>
           </c:ext>
         </c:extLst>
       </c:lineChart>
+      <c:catAx>
+        <c:axId val="135900189"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="331890220"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="331890220"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="135900189"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr lang="zh-CN"/>
+      </a:pPr>
+    </a:p>
+  </c:txPr>
+  <c:externalData r:id="rId1">
+    <c:autoUpdate val="0"/>
+  </c:externalData>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr defTabSz="914400">
+              <a:defRPr lang="zh-CN" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>LUTs Cost</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" altLang="zh-CN"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Overall LUTs V1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>66</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>543</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>578</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>636</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>691</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>783</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>956</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1083</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1491</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Overall LUTs V3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>66</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>830</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>867</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>872</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1216</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1669</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2206</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3608</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="0"/>
+        <c:axId val="135900189"/>
+        <c:axId val="331890220"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$C$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Overall LUTs V2</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent3"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:delete val="1"/>
+                </c:dLbls>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref/>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$2:$A$9</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>33</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>66</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>{830,874,880,1035,1228,1715,2431,4129}</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>830</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>874</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>880</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1035</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1228</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1715</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>2431</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>4129</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$E$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Overall FFs V1</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent4"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:delete val="1"/>
+                </c:dLbls>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref/>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$2:$A$9</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>33</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>66</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>{487,495,513,553,618,758,842,1065}</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>487</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>495</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>513</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>553</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>618</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>758</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>842</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>1065</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="4"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$F$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Overall FFs V2</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent5"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:delete val="1"/>
+                </c:dLbls>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref/>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$2:$A$9</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>33</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>66</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>{1002,1031,1046,1133,1278,1597,1918,2875}</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>1002</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1031</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1046</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1133</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1278</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1597</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>1918</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>2875</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="135900189"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="331890220"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="331890220"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="135900189"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr lang="zh-CN"/>
+      </a:pPr>
+    </a:p>
+  </c:txPr>
+  <c:externalData r:id="rId1">
+    <c:autoUpdate val="0"/>
+  </c:externalData>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr defTabSz="914400">
+              <a:defRPr lang="zh-CN" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>FFs Cost</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" altLang="zh-CN"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Overall FFs V1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>66</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>{487,495,513,553,618,758,842,1065}</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>487</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>495</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>513</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>553</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>618</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>758</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>842</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1065</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Overall FFs V3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>66</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1023</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1030</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1093</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1198</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1429</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1662</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2355</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="0"/>
+        <c:axId val="135900189"/>
+        <c:axId val="331890220"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>N</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:delete val="1"/>
+                </c:dLbls>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref/>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$2:$A$9</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>33</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>66</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>{1,2,3,6,11,22,33,66}</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>33</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>66</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Overall LUTs V1</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent2"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:delete val="1"/>
+                </c:dLbls>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref/>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$2:$A$9</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>33</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>66</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>{543,578,636,691,783,956,1083,1491}</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>543</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>578</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>636</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>691</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>783</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>956</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>1083</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>1491</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$C$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Overall LUTs V2</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent3"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:delete val="1"/>
+                </c:dLbls>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref/>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$2:$A$9</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>33</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>66</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>{830,874,880,1035,1228,1715,2431,4129}</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>830</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>874</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>880</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1035</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1228</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1715</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>2431</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>4129</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="4"/>
+                <c:order val="4"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$F$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Overall FFs V2</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent5"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:delete val="1"/>
+                </c:dLbls>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref/>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$2:$A$9</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>33</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>66</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>{1002,1031,1046,1133,1278,1597,1918,2875}</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>1002</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1031</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1046</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1133</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1278</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1597</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>1918</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>2875</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
       <c:catAx>
         <c:axId val="135900189"/>
         <c:scaling>
@@ -2428,6 +4253,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -3460,20 +5365,1052 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>434975</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>117475</xdr:rowOff>
+      <xdr:colOff>492125</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>174625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>681990</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>98425</xdr:rowOff>
+      <xdr:colOff>739140</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>155575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3481,7 +6418,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1120775" y="3013075"/>
+        <a:off x="1177925" y="4156075"/>
         <a:ext cx="7447915" cy="3781425"/>
       </xdr:xfrm>
       <a:graphic>
@@ -3495,15 +6432,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>86360</xdr:rowOff>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>181610</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>589915</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>132080</xdr:rowOff>
+      <xdr:colOff>485140</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>46355</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3511,12 +6448,72 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10363200" y="2981960"/>
-        <a:ext cx="6495415" cy="3846195"/>
+        <a:off x="10258425" y="4162425"/>
+        <a:ext cx="7886065" cy="3846830"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>799465</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="图表 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="1238250" y="8667750"/>
+        <a:ext cx="7447915" cy="3781425"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>513715</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>179705</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="图表 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="10287000" y="8639175"/>
+        <a:ext cx="7886065" cy="3846830"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3783,10 +6780,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -3798,9 +6795,13 @@
     <col min="6" max="6" width="18.125" customWidth="1"/>
     <col min="7" max="7" width="16.875" customWidth="1"/>
     <col min="8" max="8" width="12.125" customWidth="1"/>
+    <col min="10" max="10" width="15.375" customWidth="1"/>
+    <col min="11" max="11" width="13.875" customWidth="1"/>
+    <col min="12" max="12" width="12.625" customWidth="1"/>
+    <col min="13" max="13" width="12.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3828,8 +6829,14 @@
       <c r="K1" t="s">
         <v>8</v>
       </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3839,14 +6846,20 @@
       <c r="C2">
         <v>830</v>
       </c>
+      <c r="D2">
+        <v>830</v>
+      </c>
       <c r="E2">
         <v>487</v>
       </c>
       <c r="F2">
         <v>1002</v>
       </c>
+      <c r="G2">
+        <v>1002</v>
+      </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3856,22 +6869,36 @@
       <c r="C3">
         <v>874</v>
       </c>
+      <c r="D3">
+        <v>867</v>
+      </c>
       <c r="E3">
         <v>495</v>
       </c>
       <c r="F3">
         <v>1031</v>
       </c>
+      <c r="G3">
+        <v>1023</v>
+      </c>
       <c r="J3">
-        <f t="shared" ref="J3:J9" si="0">C3-C2</f>
+        <f t="shared" ref="J3:M3" si="0">C3-C2</f>
         <v>44</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K9" si="1">F3-F2</f>
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="L3">
+        <f>F3-F2</f>
         <v>29</v>
       </c>
+      <c r="M3">
+        <f>G3-G2</f>
+        <v>21</v>
+      </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3881,22 +6908,36 @@
       <c r="C4">
         <v>880</v>
       </c>
+      <c r="D4">
+        <v>872</v>
+      </c>
       <c r="E4">
         <v>513</v>
       </c>
       <c r="F4">
         <v>1046</v>
       </c>
+      <c r="G4">
+        <v>1030</v>
+      </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="J3:J9" si="1">C4-C3</f>
         <v>6</v>
       </c>
       <c r="K4">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="K4:K9" si="2">D4-D3</f>
+        <v>5</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L3:L9" si="3">F4-F3</f>
         <v>15</v>
       </c>
+      <c r="M4">
+        <f t="shared" ref="M4:M9" si="4">G4-G3</f>
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:13">
       <c r="A5">
         <v>6</v>
       </c>
@@ -3906,22 +6947,36 @@
       <c r="C5">
         <v>1035</v>
       </c>
+      <c r="D5">
+        <v>1003</v>
+      </c>
       <c r="E5">
         <v>553</v>
       </c>
       <c r="F5">
         <v>1133</v>
       </c>
+      <c r="G5">
+        <v>1093</v>
+      </c>
       <c r="J5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>155</v>
       </c>
       <c r="K5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>131</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="3"/>
         <v>87</v>
       </c>
+      <c r="M5">
+        <f t="shared" si="4"/>
+        <v>63</v>
+      </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:13">
       <c r="A6">
         <v>11</v>
       </c>
@@ -3931,22 +6986,36 @@
       <c r="C6">
         <v>1228</v>
       </c>
+      <c r="D6">
+        <v>1216</v>
+      </c>
       <c r="E6">
         <v>618</v>
       </c>
       <c r="F6">
         <v>1278</v>
       </c>
+      <c r="G6">
+        <v>1198</v>
+      </c>
       <c r="J6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>193</v>
       </c>
       <c r="K6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>213</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="3"/>
         <v>145</v>
       </c>
+      <c r="M6">
+        <f t="shared" si="4"/>
+        <v>105</v>
+      </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:13">
       <c r="A7">
         <v>22</v>
       </c>
@@ -3969,15 +7038,23 @@
         <v>1429</v>
       </c>
       <c r="J7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>487</v>
       </c>
       <c r="K7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>453</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="3"/>
         <v>319</v>
       </c>
+      <c r="M7">
+        <f t="shared" si="4"/>
+        <v>231</v>
+      </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:13">
       <c r="A8">
         <v>33</v>
       </c>
@@ -3987,22 +7064,36 @@
       <c r="C8">
         <v>2431</v>
       </c>
+      <c r="D8">
+        <v>2206</v>
+      </c>
       <c r="E8">
         <v>842</v>
       </c>
       <c r="F8">
         <v>1918</v>
       </c>
+      <c r="G8">
+        <v>1662</v>
+      </c>
       <c r="J8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>716</v>
       </c>
       <c r="K8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>537</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="3"/>
         <v>321</v>
       </c>
+      <c r="M8">
+        <f t="shared" si="4"/>
+        <v>233</v>
+      </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>66</v>
       </c>
@@ -4025,32 +7116,40 @@
         <v>2355</v>
       </c>
       <c r="J9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1698</v>
       </c>
       <c r="K9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>1402</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="3"/>
         <v>957</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="4"/>
+        <v>693</v>
       </c>
     </row>
     <row r="13" spans="2:7">
       <c r="B13" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E13" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -4074,6 +7173,83 @@
       </c>
       <c r="G14" s="1">
         <v>0.0027</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>33</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.0051</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.0019</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>22</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.0039</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.0016</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>11</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.0028</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0.0014</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.0023</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0.0013</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.002</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0.0012</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.002</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0.0012</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.0019</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0.0012</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update the dividing strategies, it now matches Anatoliy's seeker position update logic
</commit_message>
<xml_diff>
--- a/doc/report from Vivado/Util Compare Ver2.xlsx
+++ b/doc/report from Vivado/Util Compare Ver2.xlsx
@@ -13,8 +13,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Hongjiang Cai</author>
+  </authors>
+  <commentList>
+    <comment ref="N9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Hongjiang Cai:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+Seeker Position locked.No position updating logics?</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>N</t>
   </si>
@@ -28,6 +60,9 @@
     <t>Overall LUTs V3</t>
   </si>
   <si>
+    <t>Overall LUTs V4</t>
+  </si>
+  <si>
     <t>Overall FFs V1</t>
   </si>
   <si>
@@ -37,16 +72,25 @@
     <t>Overall FFs V3</t>
   </si>
   <si>
+    <t>Overall FFs V4</t>
+  </si>
+  <si>
     <t>LUTs growth V2</t>
   </si>
   <si>
     <t>LUTs growth V3</t>
   </si>
   <si>
+    <t>LUTs growth V4</t>
+  </si>
+  <si>
     <t>FFs growth V2</t>
   </si>
   <si>
     <t>FFs growth V3</t>
+  </si>
+  <si>
+    <t>FFs growth V4</t>
   </si>
   <si>
     <t>LUTs Percentage V1</t>
@@ -58,6 +102,9 @@
     <t>LUTs Percentage V3</t>
   </si>
   <si>
+    <t>LUTs Percentage V4</t>
+  </si>
+  <si>
     <t>FFs Percentage V1</t>
   </si>
   <si>
@@ -66,18 +113,21 @@
   <si>
     <t>FFs Percentage V3</t>
   </si>
+  <si>
+    <t>FFs Percentage V4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,52 +137,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -146,9 +151,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="等线"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -160,16 +173,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
@@ -184,8 +211,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
@@ -200,6 +250,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="等线"/>
@@ -209,15 +267,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -229,6 +279,17 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -239,19 +300,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -269,7 +318,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -281,7 +336,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -293,7 +360,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -305,13 +420,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -323,85 +462,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -413,7 +474,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -430,6 +491,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -451,15 +521,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -468,20 +529,39 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -501,32 +581,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -536,10 +597,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -548,19 +609,19 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -569,118 +630,119 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -993,6 +1055,103 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Overall LUTs V4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>66</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>831</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>854</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>907</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1026</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1235</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1598</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2470</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1515</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1094,34 +1253,6 @@
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="8"/>
-                      <c:pt idx="0">
-                        <c:v>830</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>874</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>880</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>1035</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>1228</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>1715</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>2431</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>4129</c:v>
-                      </c:pt>
-                    </c:numCache>
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
@@ -1136,7 +1267,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$E$1</c15:sqref>
+                          <c15:sqref>Sheet1!$F$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1210,7 +1341,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$E$2:$E$9</c15:sqref>
+                          <c15:sqref>Sheet1!$F$2:$F$9</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1256,7 +1387,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$F$1</c15:sqref>
+                          <c15:sqref>Sheet1!$G$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1330,38 +1461,10 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$F$2:$F$9</c15:sqref>
+                          <c15:sqref>Sheet1!$G$2:$G$9</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="8"/>
-                      <c:pt idx="0">
-                        <c:v>1002</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>1031</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>1046</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>1133</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>1278</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>1597</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>1918</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>2875</c:v>
-                      </c:pt>
-                    </c:numCache>
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
@@ -1611,7 +1714,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
+              <c:f>Sheet1!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1708,7 +1811,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$1</c:f>
+              <c:f>Sheet1!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1767,7 +1870,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$9</c:f>
+              <c:f>Sheet1!$H$2:$H$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1794,6 +1897,105 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2355</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Overall FFs V4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>66</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$2:$I$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1019</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1044</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1095</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1212</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1399</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1674</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1587</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2141,34 +2343,6 @@
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="8"/>
-                      <c:pt idx="0">
-                        <c:v>830</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>874</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>880</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>1035</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>1228</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>1715</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>2431</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>4129</c:v>
-                      </c:pt>
-                    </c:numCache>
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
@@ -2183,7 +2357,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$F$1</c15:sqref>
+                          <c15:sqref>Sheet1!$G$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2860,7 +3034,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$E$1</c15:sqref>
+                          <c15:sqref>Sheet1!$F$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2977,7 +3151,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$F$1</c15:sqref>
+                          <c15:sqref>Sheet1!$G$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3328,7 +3502,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
+              <c:f>Sheet1!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3422,7 +3596,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$1</c:f>
+              <c:f>Sheet1!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3479,7 +3653,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$9</c:f>
+              <c:f>Sheet1!$H$2:$H$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3885,7 +4059,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$F$1</c15:sqref>
+                          <c15:sqref>Sheet1!$G$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -6419,7 +6593,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="1177925" y="4156075"/>
-        <a:ext cx="7447915" cy="3781425"/>
+        <a:ext cx="5213350" cy="3781425"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6448,8 +6622,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10258425" y="4162425"/>
-        <a:ext cx="7886065" cy="3846830"/>
+        <a:off x="7781925" y="4162425"/>
+        <a:ext cx="7514590" cy="3846830"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6479,7 +6653,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="1238250" y="8667750"/>
-        <a:ext cx="7447915" cy="3781425"/>
+        <a:ext cx="5153025" cy="3781425"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6508,8 +6682,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10287000" y="8639175"/>
-        <a:ext cx="7886065" cy="3846830"/>
+        <a:off x="7810500" y="8639175"/>
+        <a:ext cx="7514590" cy="3846830"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6780,28 +6954,33 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H63" sqref="H63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="19.75" customWidth="1"/>
-    <col min="3" max="3" width="19.625" customWidth="1"/>
+    <col min="3" max="3" width="19.625" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="19.25" customWidth="1"/>
     <col min="5" max="5" width="17.75" customWidth="1"/>
     <col min="6" max="6" width="18.125" customWidth="1"/>
-    <col min="7" max="7" width="16.875" customWidth="1"/>
-    <col min="8" max="8" width="12.125" customWidth="1"/>
+    <col min="7" max="7" width="16.875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="16.125" customWidth="1"/>
+    <col min="9" max="9" width="15.5" customWidth="1"/>
     <col min="10" max="10" width="15.375" customWidth="1"/>
     <col min="11" max="11" width="13.875" customWidth="1"/>
-    <col min="12" max="12" width="12.625" customWidth="1"/>
-    <col min="13" max="13" width="12.375" customWidth="1"/>
+    <col min="12" max="12" width="14.375" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5" customWidth="1"/>
+    <col min="14" max="14" width="13.875" customWidth="1"/>
+    <col min="16" max="16" width="13.625" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="13.25" customWidth="1"/>
+    <col min="18" max="18" width="12.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6823,10 +7002,10 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
       <c r="L1" t="s">
@@ -6835,8 +7014,20 @@
       <c r="M1" t="s">
         <v>10</v>
       </c>
+      <c r="N1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6850,16 +7041,22 @@
         <v>830</v>
       </c>
       <c r="E2">
+        <v>831</v>
+      </c>
+      <c r="F2">
         <v>487</v>
-      </c>
-      <c r="F2">
-        <v>1002</v>
       </c>
       <c r="G2">
         <v>1002</v>
       </c>
+      <c r="H2">
+        <v>1002</v>
+      </c>
+      <c r="I2">
+        <v>1002</v>
+      </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6873,32 +7070,46 @@
         <v>867</v>
       </c>
       <c r="E3">
+        <v>854</v>
+      </c>
+      <c r="F3">
         <v>495</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>1031</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>1023</v>
       </c>
-      <c r="J3">
-        <f t="shared" ref="J3:M3" si="0">C3-C2</f>
+      <c r="I3">
+        <v>1019</v>
+      </c>
+      <c r="L3">
+        <f>C3-C2</f>
         <v>44</v>
       </c>
-      <c r="K3">
-        <f t="shared" si="0"/>
+      <c r="M3">
+        <f>D3-D2</f>
         <v>37</v>
       </c>
-      <c r="L3">
-        <f>F3-F2</f>
+      <c r="N3">
+        <f>E3-E2</f>
+        <v>23</v>
+      </c>
+      <c r="P3">
+        <f>G3-G2</f>
         <v>29</v>
       </c>
-      <c r="M3">
-        <f>G3-G2</f>
+      <c r="Q3">
+        <f>H3-H2</f>
         <v>21</v>
       </c>
+      <c r="R3">
+        <f>I3-I2</f>
+        <v>17</v>
+      </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>3</v>
       </c>
@@ -6912,32 +7123,46 @@
         <v>872</v>
       </c>
       <c r="E4">
+        <v>907</v>
+      </c>
+      <c r="F4">
         <v>513</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>1046</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>1030</v>
       </c>
-      <c r="J4">
-        <f t="shared" ref="J3:J9" si="1">C4-C3</f>
+      <c r="I4">
+        <v>1044</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L3:L9" si="0">C4-C3</f>
         <v>6</v>
       </c>
-      <c r="K4">
-        <f t="shared" ref="K4:K9" si="2">D4-D3</f>
+      <c r="M4">
+        <f t="shared" ref="M4:M9" si="1">D4-D3</f>
         <v>5</v>
       </c>
-      <c r="L4">
-        <f t="shared" ref="L3:L9" si="3">F4-F3</f>
+      <c r="N4">
+        <f>E4-E3</f>
+        <v>53</v>
+      </c>
+      <c r="P4">
+        <f t="shared" ref="P3:P9" si="2">G4-G3</f>
         <v>15</v>
       </c>
-      <c r="M4">
-        <f t="shared" ref="M4:M9" si="4">G4-G3</f>
+      <c r="Q4">
+        <f t="shared" ref="Q4:Q9" si="3">H4-H3</f>
         <v>7</v>
       </c>
+      <c r="R4">
+        <f>I4-I3</f>
+        <v>25</v>
+      </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>6</v>
       </c>
@@ -6951,32 +7176,46 @@
         <v>1003</v>
       </c>
       <c r="E5">
+        <v>1026</v>
+      </c>
+      <c r="F5">
         <v>553</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>1133</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>1093</v>
       </c>
-      <c r="J5">
+      <c r="I5">
+        <v>1095</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>155</v>
+      </c>
+      <c r="M5">
         <f t="shared" si="1"/>
-        <v>155</v>
-      </c>
-      <c r="K5">
+        <v>131</v>
+      </c>
+      <c r="N5">
+        <f>E5-E4</f>
+        <v>119</v>
+      </c>
+      <c r="P5">
         <f t="shared" si="2"/>
-        <v>131</v>
-      </c>
-      <c r="L5">
+        <v>87</v>
+      </c>
+      <c r="Q5">
         <f t="shared" si="3"/>
-        <v>87</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="4"/>
         <v>63</v>
       </c>
+      <c r="R5">
+        <f>I5-I4</f>
+        <v>51</v>
+      </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>11</v>
       </c>
@@ -6990,32 +7229,46 @@
         <v>1216</v>
       </c>
       <c r="E6">
+        <v>1235</v>
+      </c>
+      <c r="F6">
         <v>618</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>1278</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>1198</v>
       </c>
-      <c r="J6">
+      <c r="I6">
+        <v>1212</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>193</v>
+      </c>
+      <c r="M6">
         <f t="shared" si="1"/>
-        <v>193</v>
-      </c>
-      <c r="K6">
+        <v>213</v>
+      </c>
+      <c r="N6">
+        <f>E6-E5</f>
+        <v>209</v>
+      </c>
+      <c r="P6">
         <f t="shared" si="2"/>
-        <v>213</v>
-      </c>
-      <c r="L6">
+        <v>145</v>
+      </c>
+      <c r="Q6">
         <f t="shared" si="3"/>
-        <v>145</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="4"/>
         <v>105</v>
       </c>
+      <c r="R6">
+        <f>I6-I5</f>
+        <v>117</v>
+      </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>22</v>
       </c>
@@ -7029,32 +7282,46 @@
         <v>1669</v>
       </c>
       <c r="E7">
+        <v>1598</v>
+      </c>
+      <c r="F7">
         <v>758</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>1597</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>1429</v>
       </c>
-      <c r="J7">
+      <c r="I7">
+        <v>1399</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>487</v>
+      </c>
+      <c r="M7">
         <f t="shared" si="1"/>
-        <v>487</v>
-      </c>
-      <c r="K7">
+        <v>453</v>
+      </c>
+      <c r="N7">
+        <f>E7-E6</f>
+        <v>363</v>
+      </c>
+      <c r="P7">
         <f t="shared" si="2"/>
-        <v>453</v>
-      </c>
-      <c r="L7">
+        <v>319</v>
+      </c>
+      <c r="Q7">
         <f t="shared" si="3"/>
-        <v>319</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="4"/>
         <v>231</v>
       </c>
+      <c r="R7">
+        <f>I7-I6</f>
+        <v>187</v>
+      </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>33</v>
       </c>
@@ -7068,32 +7335,46 @@
         <v>2206</v>
       </c>
       <c r="E8">
+        <v>2470</v>
+      </c>
+      <c r="F8">
         <v>842</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>1918</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>1662</v>
       </c>
-      <c r="J8">
+      <c r="I8">
+        <v>1674</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>716</v>
+      </c>
+      <c r="M8">
         <f t="shared" si="1"/>
-        <v>716</v>
-      </c>
-      <c r="K8">
+        <v>537</v>
+      </c>
+      <c r="N8">
+        <f>E8-E7</f>
+        <v>872</v>
+      </c>
+      <c r="P8">
         <f t="shared" si="2"/>
-        <v>537</v>
-      </c>
-      <c r="L8">
+        <v>321</v>
+      </c>
+      <c r="Q8">
         <f t="shared" si="3"/>
-        <v>321</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="4"/>
         <v>233</v>
       </c>
+      <c r="R8">
+        <f>I8-I7</f>
+        <v>275</v>
+      </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>66</v>
       </c>
@@ -7107,52 +7388,72 @@
         <v>3608</v>
       </c>
       <c r="E9">
+        <v>1515</v>
+      </c>
+      <c r="F9">
         <v>1065</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>2875</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>2355</v>
       </c>
-      <c r="J9">
+      <c r="I9">
+        <v>1587</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>1698</v>
+      </c>
+      <c r="M9">
         <f t="shared" si="1"/>
-        <v>1698</v>
-      </c>
-      <c r="K9">
+        <v>1402</v>
+      </c>
+      <c r="N9">
+        <f>E9-E8</f>
+        <v>-955</v>
+      </c>
+      <c r="P9">
         <f t="shared" si="2"/>
-        <v>1402</v>
-      </c>
-      <c r="L9">
+        <v>957</v>
+      </c>
+      <c r="Q9">
         <f t="shared" si="3"/>
-        <v>957</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="4"/>
         <v>693</v>
       </c>
+      <c r="R9">
+        <f>I9-I8</f>
+        <v>-87</v>
+      </c>
     </row>
-    <row r="13" spans="2:7">
+    <row r="13" spans="2:9">
       <c r="B13" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E13" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F13" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G13" t="s">
-        <v>16</v>
+        <v>20</v>
+      </c>
+      <c r="H13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:9">
       <c r="A14">
         <v>66</v>
       </c>
@@ -7166,98 +7467,147 @@
         <v>0.0083</v>
       </c>
       <c r="E14" s="1">
+        <v>0.0035</v>
+      </c>
+      <c r="F14" s="1">
         <v>0.0012</v>
       </c>
-      <c r="F14" s="1">
+      <c r="G14" s="1">
         <v>0.0033</v>
       </c>
-      <c r="G14" s="1">
+      <c r="H14" s="1">
         <v>0.0027</v>
       </c>
+      <c r="I14" s="1">
+        <v>0.0018</v>
+      </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:9">
       <c r="A15">
         <v>33</v>
       </c>
       <c r="D15" s="1">
         <v>0.0051</v>
       </c>
-      <c r="G15" s="1">
+      <c r="E15" s="1">
+        <v>0.0057</v>
+      </c>
+      <c r="H15" s="1">
         <v>0.0019</v>
       </c>
+      <c r="I15" s="1">
+        <v>0.0019</v>
+      </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:9">
       <c r="A16">
         <v>22</v>
       </c>
       <c r="D16" s="1">
         <v>0.0039</v>
       </c>
-      <c r="G16" s="1">
+      <c r="E16" s="1">
+        <v>0.0037</v>
+      </c>
+      <c r="H16" s="1">
         <v>0.0016</v>
       </c>
+      <c r="I16" s="1">
+        <v>0.0016</v>
+      </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>11</v>
       </c>
       <c r="D17" s="1">
         <v>0.0028</v>
       </c>
-      <c r="G17" s="1">
+      <c r="E17" s="1">
+        <v>0.0028</v>
+      </c>
+      <c r="H17" s="1">
         <v>0.0014</v>
       </c>
+      <c r="I17" s="1">
+        <v>0.0014</v>
+      </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:9">
       <c r="A18">
         <v>6</v>
       </c>
       <c r="D18" s="1">
         <v>0.0023</v>
       </c>
-      <c r="G18" s="1">
+      <c r="E18" s="1">
+        <v>0.0024</v>
+      </c>
+      <c r="H18" s="1">
         <v>0.0013</v>
       </c>
+      <c r="I18" s="1">
+        <v>0.0013</v>
+      </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:9">
       <c r="A19">
         <v>3</v>
       </c>
       <c r="D19" s="1">
         <v>0.002</v>
       </c>
-      <c r="G19" s="1">
+      <c r="E19" s="1">
+        <v>0.0021</v>
+      </c>
+      <c r="H19" s="1">
         <v>0.0012</v>
       </c>
+      <c r="I19" s="1">
+        <v>0.0012</v>
+      </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:9">
       <c r="A20">
         <v>2</v>
       </c>
       <c r="D20" s="1">
         <v>0.002</v>
       </c>
-      <c r="G20" s="1">
+      <c r="E20" s="2">
+        <v>0.002</v>
+      </c>
+      <c r="H20" s="1">
         <v>0.0012</v>
       </c>
+      <c r="I20" s="1">
+        <v>0.0012</v>
+      </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:9">
       <c r="A21">
         <v>1</v>
       </c>
       <c r="D21" s="1">
         <v>0.0019</v>
       </c>
-      <c r="G21" s="1">
+      <c r="E21" s="1">
+        <v>0.0019</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0.0012</v>
+      </c>
+      <c r="I21" s="1">
         <v>0.0012</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F9">
+  <sortState ref="A2:G9">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new data for more N
</commit_message>
<xml_diff>
--- a/doc/report from Vivado/Util Compare Ver2.xlsx
+++ b/doc/report from Vivado/Util Compare Ver2.xlsx
@@ -19,7 +19,7 @@
     <author>Hongjiang Cai</author>
   </authors>
   <commentList>
-    <comment ref="N9" authorId="0">
+    <comment ref="Z9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>N</t>
   </si>
@@ -63,6 +63,18 @@
     <t>Overall LUTs V4</t>
   </si>
   <si>
+    <t>Overall LUTs HC's w/old project</t>
+  </si>
+  <si>
+    <t>Overall LUTs A's w/old project</t>
+  </si>
+  <si>
+    <t>Overall LUTs HC's w/new project</t>
+  </si>
+  <si>
+    <t>Overall LUTs A's w/new project</t>
+  </si>
+  <si>
     <t>Overall FFs V1</t>
   </si>
   <si>
@@ -75,7 +87,16 @@
     <t>Overall FFs V4</t>
   </si>
   <si>
-    <t>LUTs growth V2</t>
+    <t>Overall FFs HC's w/old project</t>
+  </si>
+  <si>
+    <t>Overall FFs A's w/old project</t>
+  </si>
+  <si>
+    <t>Overall FFs HC's w/new project</t>
+  </si>
+  <si>
+    <t>Overall FFs A's w/new project</t>
   </si>
   <si>
     <t>LUTs growth V3</t>
@@ -122,10 +143,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -133,6 +154,13 @@
       <color theme="1"/>
       <name val="等线"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -150,6 +178,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="等线"/>
@@ -158,10 +194,24 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -173,15 +223,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF0000FF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -195,6 +246,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -203,16 +277,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -226,55 +293,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -300,7 +321,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -312,7 +345,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -324,7 +363,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -336,55 +417,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -402,19 +441,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -432,49 +477,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -491,15 +512,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -521,8 +533,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -532,36 +544,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -583,6 +565,45 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -597,10 +618,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -609,16 +630,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -627,13 +648,13 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -642,100 +663,100 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1267,7 +1288,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$F$1</c15:sqref>
+                          <c15:sqref>Sheet1!$M$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1341,7 +1362,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$F$2:$F$9</c15:sqref>
+                          <c15:sqref>Sheet1!$M$2:$M$9</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1387,7 +1408,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$G$1</c15:sqref>
+                          <c15:sqref>Sheet1!$N$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1461,7 +1482,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$G$2:$G$9</c15:sqref>
+                          <c15:sqref>Sheet1!$N$2:$N$9</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1714,7 +1735,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$1</c:f>
+              <c:f>Sheet1!$M$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1811,7 +1832,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$1</c:f>
+              <c:f>Sheet1!$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1870,7 +1891,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$9</c:f>
+              <c:f>Sheet1!$O$2:$O$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1908,7 +1929,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$1</c:f>
+              <c:f>Sheet1!$P$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1969,7 +1990,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$9</c:f>
+              <c:f>Sheet1!$P$2:$P$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2357,7 +2378,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$G$1</c15:sqref>
+                          <c15:sqref>Sheet1!$N$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3034,7 +3055,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$F$1</c15:sqref>
+                          <c15:sqref>Sheet1!$M$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3151,7 +3172,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$G$1</c15:sqref>
+                          <c15:sqref>Sheet1!$N$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3502,7 +3523,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$1</c:f>
+              <c:f>Sheet1!$M$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3596,7 +3617,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$1</c:f>
+              <c:f>Sheet1!$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3653,7 +3674,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$9</c:f>
+              <c:f>Sheet1!$O$2:$O$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4059,7 +4080,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$G$1</c15:sqref>
+                          <c15:sqref>Sheet1!$N$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -4274,6 +4295,1464 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr lang="zh-CN"/>
+      </a:pPr>
+    </a:p>
+  </c:txPr>
+  <c:externalData r:id="rId1">
+    <c:autoUpdate val="0"/>
+  </c:externalData>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr defTabSz="914400">
+              <a:defRPr lang="zh-CN" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>Overall LUTs Cost</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" altLang="zh-CN"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.463445628075488"/>
+          <c:y val="0.0304449648711944"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Overall LUTs HC's w/old project</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>66</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>464</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>491</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>553</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>619</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>890</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1136</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1844</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>900</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Overall LUTs A's w/old project</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>66</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>544</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>579</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>637</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>692</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>784</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>957</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1084</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1493</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Overall LUTs HC's w/new project</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>66</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>832</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>855</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>908</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1027</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1235</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1599</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2471</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1516</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Overall LUTs A's w/new project</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>66</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$2:$I$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>834</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>868</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>926</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>981</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1073</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1249</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1374</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1781</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="180919255"/>
+        <c:axId val="362862828"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="180919255"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="362862828"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="362862828"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="180919255"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr lang="zh-CN"/>
+      </a:pPr>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr defTabSz="914400">
+              <a:defRPr lang="zh-CN" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>Overall FFs Cost</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" altLang="zh-CN"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.463445628075488"/>
+          <c:y val="0.0304449648711944"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Overall FFs HC's w/old project</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>66</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Q$2:$Q$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>473</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>489</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>499</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>532</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>603</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>724</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>889</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>936</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$R$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Overall FFs A's w/old project</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>66</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$2:$R$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>487</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>495</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>513</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>553</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>618</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>758</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>842</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1065</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$S$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Overall FFs HC's w/new project</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>66</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$S$2:$S$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1019</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1044</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1095</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1212</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1399</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1674</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1587</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$T$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Overall FFs A's w/new project</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>66</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$T$2:$T$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1010</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1028</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1068</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1133</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1273</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1357</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1580</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="180919255"/>
+        <c:axId val="362862828"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="180919255"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="362862828"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="362862828"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="180919255"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -4507,6 +5986,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -6571,20 +8130,1052 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>492125</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>174625</xdr:rowOff>
+      <xdr:colOff>530225</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>22225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>739140</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>155575</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>3175</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6592,8 +9183,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1177925" y="4156075"/>
-        <a:ext cx="5213350" cy="3781425"/>
+        <a:off x="1216025" y="13233400"/>
+        <a:ext cx="15557500" cy="3781425"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6605,16 +9196,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>181610</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>485140</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>46355</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>447040</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>113030</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6622,8 +9213,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7781925" y="4162425"/>
-        <a:ext cx="7514590" cy="3846830"/>
+        <a:off x="18087975" y="13096875"/>
+        <a:ext cx="15763240" cy="3846830"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6636,15 +9227,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>799465</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6652,8 +9243,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1238250" y="8667750"/>
-        <a:ext cx="5153025" cy="3781425"/>
+        <a:off x="1314450" y="17497425"/>
+        <a:ext cx="15497175" cy="3781425"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6665,15 +9256,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>95</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>513715</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>399415</xdr:colOff>
+      <xdr:row>116</xdr:row>
       <xdr:rowOff>179705</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
@@ -6682,12 +9273,72 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7810500" y="8639175"/>
-        <a:ext cx="7514590" cy="3846830"/>
+        <a:off x="18040350" y="17325975"/>
+        <a:ext cx="15763240" cy="3846830"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>98425</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>662305</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>59690</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="图表 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="2216150" y="4622800"/>
+        <a:ext cx="11743055" cy="4485640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>417830</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>27940</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="图表 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="16925925" y="4591050"/>
+        <a:ext cx="11743055" cy="4485640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6954,10 +9605,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:R21"/>
+  <dimension ref="A1:AD21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -6966,21 +9617,26 @@
     <col min="3" max="3" width="19.625" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="19.25" customWidth="1"/>
     <col min="5" max="5" width="17.75" customWidth="1"/>
-    <col min="6" max="6" width="18.125" customWidth="1"/>
-    <col min="7" max="7" width="16.875" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="16.125" customWidth="1"/>
-    <col min="9" max="9" width="15.5" customWidth="1"/>
-    <col min="10" max="10" width="15.375" customWidth="1"/>
-    <col min="11" max="11" width="13.875" customWidth="1"/>
-    <col min="12" max="12" width="14.375" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5" customWidth="1"/>
-    <col min="14" max="14" width="13.875" customWidth="1"/>
-    <col min="16" max="16" width="13.625" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="13.25" customWidth="1"/>
-    <col min="18" max="18" width="12.875" customWidth="1"/>
+    <col min="6" max="6" width="27" customWidth="1"/>
+    <col min="7" max="7" width="26.875" customWidth="1"/>
+    <col min="8" max="8" width="27.875" customWidth="1"/>
+    <col min="9" max="9" width="27" customWidth="1"/>
+    <col min="13" max="13" width="18.125" customWidth="1"/>
+    <col min="14" max="14" width="16.875" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="16.125" customWidth="1"/>
+    <col min="16" max="16" width="15.5" customWidth="1"/>
+    <col min="17" max="17" width="25.5" customWidth="1"/>
+    <col min="18" max="18" width="24.75" customWidth="1"/>
+    <col min="19" max="19" width="26.375" customWidth="1"/>
+    <col min="20" max="20" width="24.875" customWidth="1"/>
+    <col min="25" max="25" width="13.5" customWidth="1"/>
+    <col min="26" max="26" width="13.875" customWidth="1"/>
+    <col min="28" max="28" width="13.625" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="13.25" customWidth="1"/>
+    <col min="30" max="30" width="12.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:30">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7008,13 +9664,13 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
       <c r="P1" t="s">
@@ -7026,8 +9682,29 @@
       <c r="R1" t="s">
         <v>14</v>
       </c>
+      <c r="S1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:20">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7044,19 +9721,43 @@
         <v>831</v>
       </c>
       <c r="F2">
+        <v>464</v>
+      </c>
+      <c r="G2">
+        <v>544</v>
+      </c>
+      <c r="H2">
+        <v>832</v>
+      </c>
+      <c r="I2">
+        <v>834</v>
+      </c>
+      <c r="M2">
         <v>487</v>
       </c>
-      <c r="G2">
+      <c r="N2">
         <v>1002</v>
       </c>
-      <c r="H2">
+      <c r="O2">
         <v>1002</v>
       </c>
-      <c r="I2">
+      <c r="P2">
         <v>1002</v>
       </c>
+      <c r="Q2">
+        <v>473</v>
+      </c>
+      <c r="R2">
+        <v>487</v>
+      </c>
+      <c r="S2">
+        <v>1002</v>
+      </c>
+      <c r="T2">
+        <v>1002</v>
+      </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:30">
       <c r="A3">
         <v>2</v>
       </c>
@@ -7073,43 +9774,67 @@
         <v>854</v>
       </c>
       <c r="F3">
+        <v>491</v>
+      </c>
+      <c r="G3">
+        <v>579</v>
+      </c>
+      <c r="H3">
+        <v>855</v>
+      </c>
+      <c r="I3">
+        <v>868</v>
+      </c>
+      <c r="M3">
         <v>495</v>
       </c>
-      <c r="G3">
+      <c r="N3">
         <v>1031</v>
       </c>
-      <c r="H3">
+      <c r="O3">
         <v>1023</v>
       </c>
-      <c r="I3">
+      <c r="P3">
         <v>1019</v>
       </c>
-      <c r="L3">
+      <c r="Q3">
+        <v>489</v>
+      </c>
+      <c r="R3">
+        <v>495</v>
+      </c>
+      <c r="S3">
+        <v>1019</v>
+      </c>
+      <c r="T3">
+        <v>1010</v>
+      </c>
+      <c r="X3">
         <f>C3-C2</f>
         <v>44</v>
       </c>
-      <c r="M3">
+      <c r="Y3">
         <f>D3-D2</f>
         <v>37</v>
       </c>
-      <c r="N3">
-        <f>E3-E2</f>
+      <c r="Z3">
+        <f t="shared" ref="Z3:Z9" si="0">E3-E2</f>
         <v>23</v>
       </c>
-      <c r="P3">
-        <f>G3-G2</f>
+      <c r="AB3">
+        <f>N3-N2</f>
         <v>29</v>
       </c>
-      <c r="Q3">
-        <f>H3-H2</f>
+      <c r="AC3">
+        <f>O3-O2</f>
         <v>21</v>
       </c>
-      <c r="R3">
-        <f>I3-I2</f>
+      <c r="AD3">
+        <f t="shared" ref="AD3:AD9" si="1">P3-P2</f>
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:30">
       <c r="A4">
         <v>3</v>
       </c>
@@ -7126,43 +9851,67 @@
         <v>907</v>
       </c>
       <c r="F4">
+        <v>553</v>
+      </c>
+      <c r="G4">
+        <v>637</v>
+      </c>
+      <c r="H4">
+        <v>908</v>
+      </c>
+      <c r="I4">
+        <v>926</v>
+      </c>
+      <c r="M4">
         <v>513</v>
       </c>
-      <c r="G4">
+      <c r="N4">
         <v>1046</v>
       </c>
-      <c r="H4">
+      <c r="O4">
         <v>1030</v>
       </c>
-      <c r="I4">
+      <c r="P4">
         <v>1044</v>
       </c>
-      <c r="L4">
-        <f t="shared" ref="L3:L9" si="0">C4-C3</f>
+      <c r="Q4">
+        <v>499</v>
+      </c>
+      <c r="R4">
+        <v>513</v>
+      </c>
+      <c r="S4">
+        <v>1044</v>
+      </c>
+      <c r="T4">
+        <v>1028</v>
+      </c>
+      <c r="X4">
+        <f t="shared" ref="X3:X9" si="2">C4-C3</f>
         <v>6</v>
       </c>
-      <c r="M4">
-        <f t="shared" ref="M4:M9" si="1">D4-D3</f>
+      <c r="Y4">
+        <f t="shared" ref="Y4:Y9" si="3">D4-D3</f>
         <v>5</v>
       </c>
-      <c r="N4">
-        <f>E4-E3</f>
+      <c r="Z4">
+        <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="P4">
-        <f t="shared" ref="P3:P9" si="2">G4-G3</f>
+      <c r="AB4">
+        <f t="shared" ref="AB3:AB9" si="4">N4-N3</f>
         <v>15</v>
       </c>
-      <c r="Q4">
-        <f t="shared" ref="Q4:Q9" si="3">H4-H3</f>
+      <c r="AC4">
+        <f t="shared" ref="AC4:AC9" si="5">O4-O3</f>
         <v>7</v>
       </c>
-      <c r="R4">
-        <f>I4-I3</f>
+      <c r="AD4">
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:30">
       <c r="A5">
         <v>6</v>
       </c>
@@ -7179,43 +9928,67 @@
         <v>1026</v>
       </c>
       <c r="F5">
+        <v>619</v>
+      </c>
+      <c r="G5">
+        <v>692</v>
+      </c>
+      <c r="H5">
+        <v>1027</v>
+      </c>
+      <c r="I5">
+        <v>981</v>
+      </c>
+      <c r="M5">
         <v>553</v>
       </c>
-      <c r="G5">
+      <c r="N5">
         <v>1133</v>
       </c>
-      <c r="H5">
+      <c r="O5">
         <v>1093</v>
       </c>
-      <c r="I5">
+      <c r="P5">
         <v>1095</v>
       </c>
-      <c r="L5">
+      <c r="Q5">
+        <v>532</v>
+      </c>
+      <c r="R5">
+        <v>553</v>
+      </c>
+      <c r="S5">
+        <v>1095</v>
+      </c>
+      <c r="T5">
+        <v>1068</v>
+      </c>
+      <c r="X5">
+        <f t="shared" si="2"/>
+        <v>155</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" si="3"/>
+        <v>131</v>
+      </c>
+      <c r="Z5">
         <f t="shared" si="0"/>
-        <v>155</v>
-      </c>
-      <c r="M5">
+        <v>119</v>
+      </c>
+      <c r="AB5">
+        <f t="shared" si="4"/>
+        <v>87</v>
+      </c>
+      <c r="AC5">
+        <f t="shared" si="5"/>
+        <v>63</v>
+      </c>
+      <c r="AD5">
         <f t="shared" si="1"/>
-        <v>131</v>
-      </c>
-      <c r="N5">
-        <f>E5-E4</f>
-        <v>119</v>
-      </c>
-      <c r="P5">
-        <f t="shared" si="2"/>
-        <v>87</v>
-      </c>
-      <c r="Q5">
-        <f t="shared" si="3"/>
-        <v>63</v>
-      </c>
-      <c r="R5">
-        <f>I5-I4</f>
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:30">
       <c r="A6">
         <v>11</v>
       </c>
@@ -7232,43 +10005,67 @@
         <v>1235</v>
       </c>
       <c r="F6">
+        <v>890</v>
+      </c>
+      <c r="G6">
+        <v>784</v>
+      </c>
+      <c r="H6">
+        <v>1235</v>
+      </c>
+      <c r="I6">
+        <v>1073</v>
+      </c>
+      <c r="M6">
         <v>618</v>
       </c>
-      <c r="G6">
+      <c r="N6">
         <v>1278</v>
       </c>
-      <c r="H6">
+      <c r="O6">
         <v>1198</v>
       </c>
-      <c r="I6">
+      <c r="P6">
         <v>1212</v>
       </c>
-      <c r="L6">
+      <c r="Q6">
+        <v>603</v>
+      </c>
+      <c r="R6">
+        <v>618</v>
+      </c>
+      <c r="S6">
+        <v>1212</v>
+      </c>
+      <c r="T6">
+        <v>1133</v>
+      </c>
+      <c r="X6">
+        <f t="shared" si="2"/>
+        <v>193</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" si="3"/>
+        <v>213</v>
+      </c>
+      <c r="Z6">
         <f t="shared" si="0"/>
-        <v>193</v>
-      </c>
-      <c r="M6">
+        <v>209</v>
+      </c>
+      <c r="AB6">
+        <f t="shared" si="4"/>
+        <v>145</v>
+      </c>
+      <c r="AC6">
+        <f t="shared" si="5"/>
+        <v>105</v>
+      </c>
+      <c r="AD6">
         <f t="shared" si="1"/>
-        <v>213</v>
-      </c>
-      <c r="N6">
-        <f>E6-E5</f>
-        <v>209</v>
-      </c>
-      <c r="P6">
-        <f t="shared" si="2"/>
-        <v>145</v>
-      </c>
-      <c r="Q6">
-        <f t="shared" si="3"/>
-        <v>105</v>
-      </c>
-      <c r="R6">
-        <f>I6-I5</f>
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:30">
       <c r="A7">
         <v>22</v>
       </c>
@@ -7285,43 +10082,67 @@
         <v>1598</v>
       </c>
       <c r="F7">
+        <v>1136</v>
+      </c>
+      <c r="G7">
+        <v>957</v>
+      </c>
+      <c r="H7">
+        <v>1599</v>
+      </c>
+      <c r="I7">
+        <v>1249</v>
+      </c>
+      <c r="M7">
         <v>758</v>
       </c>
-      <c r="G7">
+      <c r="N7">
         <v>1597</v>
       </c>
-      <c r="H7">
+      <c r="O7">
         <v>1429</v>
       </c>
-      <c r="I7">
+      <c r="P7">
         <v>1399</v>
       </c>
-      <c r="L7">
+      <c r="Q7">
+        <v>724</v>
+      </c>
+      <c r="R7">
+        <v>758</v>
+      </c>
+      <c r="S7">
+        <v>1399</v>
+      </c>
+      <c r="T7">
+        <v>1273</v>
+      </c>
+      <c r="X7">
+        <f t="shared" si="2"/>
+        <v>487</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" si="3"/>
+        <v>453</v>
+      </c>
+      <c r="Z7">
         <f t="shared" si="0"/>
-        <v>487</v>
-      </c>
-      <c r="M7">
+        <v>363</v>
+      </c>
+      <c r="AB7">
+        <f t="shared" si="4"/>
+        <v>319</v>
+      </c>
+      <c r="AC7">
+        <f t="shared" si="5"/>
+        <v>231</v>
+      </c>
+      <c r="AD7">
         <f t="shared" si="1"/>
-        <v>453</v>
-      </c>
-      <c r="N7">
-        <f>E7-E6</f>
-        <v>363</v>
-      </c>
-      <c r="P7">
-        <f t="shared" si="2"/>
-        <v>319</v>
-      </c>
-      <c r="Q7">
-        <f t="shared" si="3"/>
-        <v>231</v>
-      </c>
-      <c r="R7">
-        <f>I7-I6</f>
         <v>187</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:30">
       <c r="A8">
         <v>33</v>
       </c>
@@ -7338,43 +10159,67 @@
         <v>2470</v>
       </c>
       <c r="F8">
+        <v>1844</v>
+      </c>
+      <c r="G8">
+        <v>1084</v>
+      </c>
+      <c r="H8">
+        <v>2471</v>
+      </c>
+      <c r="I8">
+        <v>1374</v>
+      </c>
+      <c r="M8">
         <v>842</v>
       </c>
-      <c r="G8">
+      <c r="N8">
         <v>1918</v>
       </c>
-      <c r="H8">
+      <c r="O8">
         <v>1662</v>
       </c>
-      <c r="I8">
+      <c r="P8">
         <v>1674</v>
       </c>
-      <c r="L8">
+      <c r="Q8">
+        <v>889</v>
+      </c>
+      <c r="R8">
+        <v>842</v>
+      </c>
+      <c r="S8">
+        <v>1674</v>
+      </c>
+      <c r="T8">
+        <v>1357</v>
+      </c>
+      <c r="X8">
+        <f t="shared" si="2"/>
+        <v>716</v>
+      </c>
+      <c r="Y8">
+        <f t="shared" si="3"/>
+        <v>537</v>
+      </c>
+      <c r="Z8">
         <f t="shared" si="0"/>
-        <v>716</v>
-      </c>
-      <c r="M8">
+        <v>872</v>
+      </c>
+      <c r="AB8">
+        <f t="shared" si="4"/>
+        <v>321</v>
+      </c>
+      <c r="AC8">
+        <f t="shared" si="5"/>
+        <v>233</v>
+      </c>
+      <c r="AD8">
         <f t="shared" si="1"/>
-        <v>537</v>
-      </c>
-      <c r="N8">
-        <f>E8-E7</f>
-        <v>872</v>
-      </c>
-      <c r="P8">
-        <f t="shared" si="2"/>
-        <v>321</v>
-      </c>
-      <c r="Q8">
-        <f t="shared" si="3"/>
-        <v>233</v>
-      </c>
-      <c r="R8">
-        <f>I8-I7</f>
         <v>275</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:30">
       <c r="A9">
         <v>66</v>
       </c>
@@ -7391,69 +10236,93 @@
         <v>1515</v>
       </c>
       <c r="F9">
+        <v>900</v>
+      </c>
+      <c r="G9">
+        <v>1493</v>
+      </c>
+      <c r="H9">
+        <v>1516</v>
+      </c>
+      <c r="I9">
+        <v>1781</v>
+      </c>
+      <c r="M9">
         <v>1065</v>
       </c>
-      <c r="G9">
+      <c r="N9">
         <v>2875</v>
       </c>
-      <c r="H9">
+      <c r="O9">
         <v>2355</v>
       </c>
-      <c r="I9">
+      <c r="P9">
         <v>1587</v>
       </c>
-      <c r="L9">
+      <c r="Q9">
+        <v>936</v>
+      </c>
+      <c r="R9">
+        <v>1065</v>
+      </c>
+      <c r="S9">
+        <v>1587</v>
+      </c>
+      <c r="T9">
+        <v>1580</v>
+      </c>
+      <c r="X9">
+        <f t="shared" si="2"/>
+        <v>1698</v>
+      </c>
+      <c r="Y9">
+        <f t="shared" si="3"/>
+        <v>1402</v>
+      </c>
+      <c r="Z9">
         <f t="shared" si="0"/>
-        <v>1698</v>
-      </c>
-      <c r="M9">
+        <v>-955</v>
+      </c>
+      <c r="AB9">
+        <f t="shared" si="4"/>
+        <v>957</v>
+      </c>
+      <c r="AC9">
+        <f t="shared" si="5"/>
+        <v>693</v>
+      </c>
+      <c r="AD9">
         <f t="shared" si="1"/>
-        <v>1402</v>
-      </c>
-      <c r="N9">
-        <f>E9-E8</f>
-        <v>-955</v>
-      </c>
-      <c r="P9">
-        <f t="shared" si="2"/>
-        <v>957</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" si="3"/>
-        <v>693</v>
-      </c>
-      <c r="R9">
-        <f>I9-I8</f>
         <v>-87</v>
       </c>
     </row>
-    <row r="13" spans="2:9">
+    <row r="13" spans="2:16">
       <c r="B13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" t="s">
-        <v>21</v>
-      </c>
-      <c r="I13" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="M13" t="s">
+        <v>26</v>
+      </c>
+      <c r="N13" t="s">
+        <v>27</v>
+      </c>
+      <c r="O13" t="s">
+        <v>28</v>
+      </c>
+      <c r="P13" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:16">
       <c r="A14">
         <v>66</v>
       </c>
@@ -7469,20 +10338,20 @@
       <c r="E14" s="1">
         <v>0.0035</v>
       </c>
-      <c r="F14" s="1">
+      <c r="M14" s="1">
         <v>0.0012</v>
       </c>
-      <c r="G14" s="1">
+      <c r="N14" s="1">
         <v>0.0033</v>
       </c>
-      <c r="H14" s="1">
+      <c r="O14" s="1">
         <v>0.0027</v>
       </c>
-      <c r="I14" s="1">
+      <c r="P14" s="1">
         <v>0.0018</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:16">
       <c r="A15">
         <v>33</v>
       </c>
@@ -7492,14 +10361,14 @@
       <c r="E15" s="1">
         <v>0.0057</v>
       </c>
-      <c r="H15" s="1">
+      <c r="O15" s="1">
         <v>0.0019</v>
       </c>
-      <c r="I15" s="1">
+      <c r="P15" s="1">
         <v>0.0019</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:16">
       <c r="A16">
         <v>22</v>
       </c>
@@ -7509,14 +10378,14 @@
       <c r="E16" s="1">
         <v>0.0037</v>
       </c>
-      <c r="H16" s="1">
+      <c r="O16" s="1">
         <v>0.0016</v>
       </c>
-      <c r="I16" s="1">
+      <c r="P16" s="1">
         <v>0.0016</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:16">
       <c r="A17">
         <v>11</v>
       </c>
@@ -7526,14 +10395,14 @@
       <c r="E17" s="1">
         <v>0.0028</v>
       </c>
-      <c r="H17" s="1">
+      <c r="O17" s="1">
         <v>0.0014</v>
       </c>
-      <c r="I17" s="1">
+      <c r="P17" s="1">
         <v>0.0014</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:16">
       <c r="A18">
         <v>6</v>
       </c>
@@ -7543,14 +10412,14 @@
       <c r="E18" s="1">
         <v>0.0024</v>
       </c>
-      <c r="H18" s="1">
+      <c r="O18" s="1">
         <v>0.0013</v>
       </c>
-      <c r="I18" s="1">
+      <c r="P18" s="1">
         <v>0.0013</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:16">
       <c r="A19">
         <v>3</v>
       </c>
@@ -7560,14 +10429,14 @@
       <c r="E19" s="1">
         <v>0.0021</v>
       </c>
-      <c r="H19" s="1">
+      <c r="O19" s="1">
         <v>0.0012</v>
       </c>
-      <c r="I19" s="1">
+      <c r="P19" s="1">
         <v>0.0012</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:16">
       <c r="A20">
         <v>2</v>
       </c>
@@ -7577,14 +10446,14 @@
       <c r="E20" s="2">
         <v>0.002</v>
       </c>
-      <c r="H20" s="1">
+      <c r="O20" s="1">
         <v>0.0012</v>
       </c>
-      <c r="I20" s="1">
+      <c r="P20" s="1">
         <v>0.0012</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:16">
       <c r="A21">
         <v>1</v>
       </c>
@@ -7594,15 +10463,15 @@
       <c r="E21" s="1">
         <v>0.0019</v>
       </c>
-      <c r="H21" s="1">
+      <c r="O21" s="1">
         <v>0.0012</v>
       </c>
-      <c r="I21" s="1">
+      <c r="P21" s="1">
         <v>0.0012</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G9">
+  <sortState ref="A2:N9">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>